<commit_message>
update script and tables
</commit_message>
<xml_diff>
--- a/Tables_v1.xlsx
+++ b/Tables_v1.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jgippet\Documents\Tmagnum_impacts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE78E748-E975-4EE2-847A-3C42B2C0EF0B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1859F397-C8AF-4C74-9C00-A498E30A47FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-8325" windowWidth="15600" windowHeight="18840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-8325" windowWidth="15600" windowHeight="18840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="26">
   <si>
     <t>Lasius niger</t>
   </si>
@@ -68,20 +69,27 @@
     <t>Tetramorium sp.</t>
   </si>
   <si>
-    <t>0.26 (0.02)</t>
-  </si>
-  <si>
-    <t>0.17 (0.07)</t>
-  </si>
-  <si>
-    <t>0.09 (0.06)</t>
-  </si>
-  <si>
     <t>0.15 (0.01)</t>
   </si>
   <si>
+    <t>Probability of foraging on bait</t>
+  </si>
+  <si>
+    <t>Number of workers recruited on bait</t>
+  </si>
+  <si>
+    <t>0.1 (0.01)</t>
+  </si>
+  <si>
     <r>
-      <t xml:space="preserve">    Pseudo-R²    </t>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Pseudo-R² </t>
     </r>
     <r>
       <rPr>
@@ -90,24 +98,46 @@
         <rFont val="Segoe UI"/>
         <family val="2"/>
       </rPr>
-      <t>(fixed effects only)</t>
+      <t xml:space="preserve">
+(fixed effects only)</t>
     </r>
   </si>
   <si>
-    <t>0.08 (0.04)</t>
-  </si>
-  <si>
-    <t>Probability of foraging on bait</t>
-  </si>
-  <si>
-    <t>Number of workers recruited on bait</t>
+    <t>0.17 (0.06)</t>
+  </si>
+  <si>
+    <t>0.1 (0.04)</t>
+  </si>
+  <si>
+    <t>0.1 (0.06)</t>
+  </si>
+  <si>
+    <t>L. niger</t>
+  </si>
+  <si>
+    <t>M. specioides</t>
+  </si>
+  <si>
+    <t>M. sabuleti</t>
+  </si>
+  <si>
+    <t>Non-invaded sites</t>
+  </si>
+  <si>
+    <t>Invaded sites</t>
+  </si>
+  <si>
+    <t>Other species</t>
+  </si>
+  <si>
+    <t>T. magnum</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -194,8 +224,77 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="6"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="9"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -214,8 +313,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="32">
+  <borders count="60">
     <border>
       <left/>
       <right/>
@@ -246,45 +357,6 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
       <top style="medium">
         <color indexed="64"/>
       </top>
@@ -558,19 +630,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="hair">
         <color indexed="64"/>
       </left>
@@ -613,6 +672,438 @@
         <color indexed="64"/>
       </right>
       <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="double">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="double">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="double">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="double">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom style="medium">
@@ -624,141 +1115,268 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="103">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1083,10 +1701,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A4:P12"/>
+  <dimension ref="A1:R12"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="R7" sqref="R7"/>
+    <sheetView showGridLines="0" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.8" x14ac:dyDescent="0.4"/>
@@ -1094,212 +1712,692 @@
     <col min="1" max="1" width="2.21875" style="1" customWidth="1"/>
     <col min="2" max="2" width="20" style="1" customWidth="1"/>
     <col min="3" max="8" width="2.6640625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="0.44140625" style="1" customWidth="1"/>
-    <col min="10" max="15" width="2.6640625" style="1" customWidth="1"/>
-    <col min="16" max="16" width="13.5546875" style="1" customWidth="1"/>
-    <col min="17" max="17" width="2.21875" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="8.88671875" style="1"/>
+    <col min="9" max="9" width="6.77734375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="0.44140625" style="1" customWidth="1"/>
+    <col min="11" max="16" width="2.6640625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="6.77734375" style="1" customWidth="1"/>
+    <col min="18" max="18" width="2.21875" style="1" customWidth="1"/>
+    <col min="19" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:16" ht="16.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
+      <c r="G1" s="52"/>
+      <c r="H1" s="52"/>
+      <c r="I1" s="52"/>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="B2" s="3"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="52"/>
+      <c r="H2" s="52"/>
+      <c r="I2" s="52"/>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="B3" s="3"/>
+      <c r="C3" s="52"/>
+      <c r="D3" s="52"/>
+      <c r="E3" s="52"/>
+      <c r="F3" s="52"/>
+      <c r="G3" s="52"/>
+      <c r="H3" s="52"/>
+      <c r="I3" s="52"/>
+    </row>
+    <row r="4" spans="1:18" ht="16.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="C4" s="53"/>
+      <c r="D4" s="53"/>
+      <c r="E4" s="53"/>
+      <c r="F4" s="53"/>
+      <c r="G4" s="53"/>
+      <c r="H4" s="53"/>
+      <c r="I4" s="53"/>
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
       <c r="M4" s="3"/>
       <c r="N4" s="3"/>
       <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="3"/>
     </row>
-    <row r="5" spans="1:16" ht="32.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C5" s="52" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="53"/>
-      <c r="E5" s="53"/>
-      <c r="F5" s="53"/>
-      <c r="G5" s="53"/>
-      <c r="H5" s="54"/>
-      <c r="I5" s="44"/>
-      <c r="J5" s="52" t="s">
-        <v>18</v>
-      </c>
-      <c r="K5" s="53"/>
-      <c r="L5" s="53"/>
-      <c r="M5" s="53"/>
-      <c r="N5" s="53"/>
-      <c r="O5" s="54"/>
+    <row r="5" spans="1:18" ht="32.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="C5" s="45" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="46"/>
+      <c r="E5" s="46"/>
+      <c r="F5" s="46"/>
+      <c r="G5" s="46"/>
+      <c r="H5" s="46"/>
+      <c r="I5" s="47"/>
+      <c r="J5" s="49"/>
+      <c r="K5" s="45" t="s">
+        <v>13</v>
+      </c>
+      <c r="L5" s="46"/>
+      <c r="M5" s="46"/>
+      <c r="N5" s="46"/>
+      <c r="O5" s="46"/>
+      <c r="P5" s="46"/>
+      <c r="Q5" s="47"/>
     </row>
-    <row r="6" spans="1:16" ht="98.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A6" s="50"/>
-      <c r="B6" s="51"/>
-      <c r="C6" s="41" t="s">
+    <row r="6" spans="1:18" ht="98.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A6" s="43"/>
+      <c r="B6" s="44"/>
+      <c r="C6" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="42" t="s">
+      <c r="D6" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="37" t="s">
+      <c r="E6" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="F6" s="43" t="s">
+      <c r="F6" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="G6" s="39" t="s">
+      <c r="G6" s="58" t="s">
         <v>5</v>
       </c>
-      <c r="H6" s="42" t="s">
+      <c r="H6" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="I6" s="47"/>
-      <c r="J6" s="36" t="s">
+      <c r="I6" s="59" t="s">
+        <v>15</v>
+      </c>
+      <c r="J6" s="35"/>
+      <c r="K6" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="K6" s="37" t="s">
+      <c r="L6" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="L6" s="38" t="s">
+      <c r="M6" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="M6" s="39" t="s">
+      <c r="N6" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="N6" s="39" t="s">
+      <c r="O6" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="O6" s="40" t="s">
+      <c r="P6" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="P6" s="11" t="s">
+      <c r="Q6" s="59" t="s">
         <v>15</v>
       </c>
+      <c r="R6" s="60"/>
     </row>
-    <row r="7" spans="1:16" s="2" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:18" s="2" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A7" s="4"/>
       <c r="B7" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="15"/>
-      <c r="D7" s="23"/>
-      <c r="E7" s="19"/>
-      <c r="F7" s="24"/>
-      <c r="G7" s="24"/>
-      <c r="H7" s="31"/>
-      <c r="I7" s="46"/>
-      <c r="J7" s="33"/>
-      <c r="K7" s="19"/>
-      <c r="L7" s="23"/>
-      <c r="M7" s="24"/>
-      <c r="N7" s="24"/>
-      <c r="O7" s="28"/>
-      <c r="P7" s="12" t="s">
+      <c r="C7" s="11"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="26"/>
+      <c r="I7" s="62"/>
+      <c r="J7" s="48"/>
+      <c r="K7" s="28"/>
+      <c r="L7" s="15"/>
+      <c r="M7" s="19"/>
+      <c r="N7" s="20"/>
+      <c r="O7" s="20"/>
+      <c r="P7" s="24"/>
+      <c r="Q7" s="66" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:16" s="2" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:18" s="2" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A8" s="4"/>
       <c r="B8" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="16"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="27"/>
-      <c r="G8" s="20"/>
-      <c r="H8" s="32"/>
-      <c r="I8" s="46"/>
-      <c r="J8" s="34"/>
-      <c r="K8" s="20"/>
-      <c r="L8" s="20"/>
-      <c r="M8" s="20"/>
-      <c r="N8" s="27"/>
-      <c r="O8" s="59"/>
-      <c r="P8" s="13" t="s">
-        <v>13</v>
+      <c r="C8" s="12"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="27"/>
+      <c r="I8" s="63"/>
+      <c r="J8" s="48"/>
+      <c r="K8" s="29"/>
+      <c r="L8" s="16"/>
+      <c r="M8" s="16"/>
+      <c r="N8" s="16"/>
+      <c r="O8" s="23"/>
+      <c r="P8" s="42"/>
+      <c r="Q8" s="65" t="s">
+        <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A9" s="5"/>
       <c r="B9" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="18"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="25"/>
-      <c r="G9" s="25"/>
-      <c r="H9" s="49"/>
-      <c r="I9" s="45"/>
-      <c r="J9" s="55"/>
-      <c r="K9" s="25"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="21"/>
+      <c r="G9" s="21"/>
+      <c r="H9" s="37"/>
+      <c r="I9" s="64"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="38"/>
       <c r="L9" s="21"/>
-      <c r="M9" s="25"/>
-      <c r="N9" s="27"/>
-      <c r="O9" s="29"/>
-      <c r="P9" s="13" t="s">
-        <v>16</v>
+      <c r="M9" s="17"/>
+      <c r="N9" s="21"/>
+      <c r="O9" s="23"/>
+      <c r="P9" s="50"/>
+      <c r="Q9" s="65" t="s">
+        <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A10" s="5"/>
       <c r="B10" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="18"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="25"/>
-      <c r="G10" s="25"/>
-      <c r="H10" s="56"/>
-      <c r="I10" s="45"/>
-      <c r="J10" s="17"/>
-      <c r="K10" s="25"/>
-      <c r="L10" s="25"/>
-      <c r="M10" s="25"/>
-      <c r="N10" s="25"/>
-      <c r="O10" s="29"/>
-      <c r="P10" s="13" t="s">
-        <v>12</v>
+      <c r="C10" s="14"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="21"/>
+      <c r="G10" s="21"/>
+      <c r="H10" s="39"/>
+      <c r="I10" s="64"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="13"/>
+      <c r="L10" s="21"/>
+      <c r="M10" s="21"/>
+      <c r="N10" s="21"/>
+      <c r="O10" s="21"/>
+      <c r="P10" s="39"/>
+      <c r="Q10" s="65" t="s">
+        <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:16" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:18" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A11" s="5"/>
       <c r="B11" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="57"/>
-      <c r="D11" s="26"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="26"/>
-      <c r="G11" s="26"/>
-      <c r="H11" s="48"/>
-      <c r="I11" s="35"/>
-      <c r="J11" s="58"/>
-      <c r="K11" s="22"/>
-      <c r="L11" s="26"/>
-      <c r="M11" s="26"/>
-      <c r="N11" s="26"/>
-      <c r="O11" s="30"/>
-      <c r="P11" s="14" t="s">
+      <c r="C11" s="40"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="36"/>
+      <c r="I11" s="61"/>
+      <c r="J11" s="25"/>
+      <c r="K11" s="41"/>
+      <c r="L11" s="18"/>
+      <c r="M11" s="22"/>
+      <c r="N11" s="22"/>
+      <c r="O11" s="22"/>
+      <c r="P11" s="51"/>
+      <c r="Q11" s="65" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.4">
       <c r="B12" s="3"/>
-      <c r="L12" s="3"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="M12" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C5:H5"/>
-    <mergeCell ref="J5:O5"/>
+    <mergeCell ref="K5:Q5"/>
+    <mergeCell ref="C5:I5"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{174BE593-B72A-41F8-A77C-9DBD61C1AADF}">
+  <dimension ref="B3:L26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6:G6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="8.88671875" style="67"/>
+    <col min="2" max="2" width="16.6640625" style="67" customWidth="1"/>
+    <col min="3" max="12" width="14.21875" style="67" customWidth="1"/>
+    <col min="13" max="16384" width="8.88671875" style="67"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="4" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C4" s="68" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="69"/>
+      <c r="E4" s="69"/>
+      <c r="F4" s="69"/>
+      <c r="G4" s="70"/>
+      <c r="H4" s="71" t="s">
+        <v>23</v>
+      </c>
+      <c r="I4" s="72"/>
+      <c r="J4" s="72"/>
+      <c r="K4" s="72"/>
+      <c r="L4" s="73"/>
+    </row>
+    <row r="5" spans="2:12" s="74" customFormat="1" ht="12" x14ac:dyDescent="0.3">
+      <c r="C5" s="75" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="76" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="76" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" s="76" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="77" t="s">
+        <v>24</v>
+      </c>
+      <c r="H5" s="78" t="s">
+        <v>19</v>
+      </c>
+      <c r="I5" s="76" t="s">
+        <v>20</v>
+      </c>
+      <c r="J5" s="76" t="s">
+        <v>21</v>
+      </c>
+      <c r="K5" s="76" t="s">
+        <v>10</v>
+      </c>
+      <c r="L5" s="79" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" ht="18" x14ac:dyDescent="0.3">
+      <c r="B6" s="80" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="99">
+        <v>267</v>
+      </c>
+      <c r="D6" s="84">
+        <v>25</v>
+      </c>
+      <c r="E6" s="84">
+        <v>0</v>
+      </c>
+      <c r="F6" s="84">
+        <v>1</v>
+      </c>
+      <c r="G6" s="85">
+        <v>6</v>
+      </c>
+      <c r="H6" s="98">
+        <v>257</v>
+      </c>
+      <c r="I6" s="84">
+        <v>13</v>
+      </c>
+      <c r="J6" s="84">
+        <v>2</v>
+      </c>
+      <c r="K6" s="84">
+        <v>1</v>
+      </c>
+      <c r="L6" s="87">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" ht="18" x14ac:dyDescent="0.3">
+      <c r="B7" s="80" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="83">
+        <v>25</v>
+      </c>
+      <c r="D7" s="97">
+        <v>66</v>
+      </c>
+      <c r="E7" s="84">
+        <v>1</v>
+      </c>
+      <c r="F7" s="84">
+        <v>0</v>
+      </c>
+      <c r="G7" s="85">
+        <v>3</v>
+      </c>
+      <c r="H7" s="86">
+        <v>13</v>
+      </c>
+      <c r="I7" s="97">
+        <v>15</v>
+      </c>
+      <c r="J7" s="84">
+        <v>0</v>
+      </c>
+      <c r="K7" s="84">
+        <v>0</v>
+      </c>
+      <c r="L7" s="87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" ht="18" x14ac:dyDescent="0.3">
+      <c r="B8" s="80" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="83">
+        <v>0</v>
+      </c>
+      <c r="D8" s="84">
+        <v>1</v>
+      </c>
+      <c r="E8" s="97">
+        <v>71</v>
+      </c>
+      <c r="F8" s="84">
+        <v>0</v>
+      </c>
+      <c r="G8" s="85">
+        <v>2</v>
+      </c>
+      <c r="H8" s="86">
+        <v>2</v>
+      </c>
+      <c r="I8" s="84">
+        <v>0</v>
+      </c>
+      <c r="J8" s="97">
+        <v>7</v>
+      </c>
+      <c r="K8" s="84">
+        <v>0</v>
+      </c>
+      <c r="L8" s="87">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="81" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="88">
+        <v>1</v>
+      </c>
+      <c r="D9" s="89">
+        <v>0</v>
+      </c>
+      <c r="E9" s="89">
+        <v>0</v>
+      </c>
+      <c r="F9" s="96">
+        <v>58</v>
+      </c>
+      <c r="G9" s="90">
+        <v>1</v>
+      </c>
+      <c r="H9" s="91">
+        <v>1</v>
+      </c>
+      <c r="I9" s="89">
+        <v>0</v>
+      </c>
+      <c r="J9" s="89">
+        <v>0</v>
+      </c>
+      <c r="K9" s="96">
+        <v>15</v>
+      </c>
+      <c r="L9" s="92">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="82" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="93"/>
+      <c r="D10" s="94"/>
+      <c r="E10" s="94"/>
+      <c r="F10" s="94"/>
+      <c r="G10" s="95"/>
+      <c r="H10" s="100">
+        <v>8</v>
+      </c>
+      <c r="I10" s="101">
+        <v>8</v>
+      </c>
+      <c r="J10" s="101">
+        <v>1</v>
+      </c>
+      <c r="K10" s="101">
+        <v>0</v>
+      </c>
+      <c r="L10" s="102">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="C14" s="67">
+        <f>ROUND(C6/960,2)</f>
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="D14" s="67">
+        <f t="shared" ref="D14:G14" si="0">ROUND(D6/960,2)</f>
+        <v>0.03</v>
+      </c>
+      <c r="E14" s="67">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F14" s="67">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G14" s="67">
+        <f t="shared" si="0"/>
+        <v>0.01</v>
+      </c>
+      <c r="H14" s="67">
+        <f>ROUND(H6/960,2)</f>
+        <v>0.27</v>
+      </c>
+      <c r="I14" s="67">
+        <f t="shared" ref="I14:L14" si="1">ROUND(I6/960,2)</f>
+        <v>0.01</v>
+      </c>
+      <c r="J14" s="67">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K14" s="67">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L14" s="67">
+        <f t="shared" si="1"/>
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="C15" s="67">
+        <f t="shared" ref="C15:G15" si="2">ROUND(C7/960,2)</f>
+        <v>0.03</v>
+      </c>
+      <c r="D15" s="67">
+        <f t="shared" si="2"/>
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="E15" s="67">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F15" s="67">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G15" s="67">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H15" s="67">
+        <f t="shared" ref="H15:L15" si="3">ROUND(H7/960,2)</f>
+        <v>0.01</v>
+      </c>
+      <c r="I15" s="67">
+        <f t="shared" si="3"/>
+        <v>0.02</v>
+      </c>
+      <c r="J15" s="67">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K15" s="67">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L15" s="67">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="C16" s="67">
+        <f t="shared" ref="C16:G16" si="4">ROUND(C8/960,2)</f>
+        <v>0</v>
+      </c>
+      <c r="D16" s="67">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="E16" s="67">
+        <f t="shared" si="4"/>
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="F16" s="67">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G16" s="67">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="H16" s="67">
+        <f t="shared" ref="H16:L16" si="5">ROUND(H8/960,2)</f>
+        <v>0</v>
+      </c>
+      <c r="I16" s="67">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J16" s="67">
+        <f t="shared" si="5"/>
+        <v>0.01</v>
+      </c>
+      <c r="K16" s="67">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="L16" s="67">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C17" s="67">
+        <f t="shared" ref="C17:G17" si="6">ROUND(C9/960,2)</f>
+        <v>0</v>
+      </c>
+      <c r="D17" s="67">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="E17" s="67">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="F17" s="67">
+        <f t="shared" si="6"/>
+        <v>0.06</v>
+      </c>
+      <c r="G17" s="67">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="H17" s="67">
+        <f t="shared" ref="H17:L18" si="7">ROUND(H9/960,2)</f>
+        <v>0</v>
+      </c>
+      <c r="I17" s="67">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="J17" s="67">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="K17" s="67">
+        <f t="shared" si="7"/>
+        <v>0.02</v>
+      </c>
+      <c r="L17" s="67">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="H18" s="67">
+        <f>ROUND(H10/960,2)</f>
+        <v>0.01</v>
+      </c>
+      <c r="I18" s="67">
+        <f t="shared" si="7"/>
+        <v>0.01</v>
+      </c>
+      <c r="J18" s="67">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="K18" s="67">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="L18" s="67">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="3:12" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="23" spans="3:12" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="24" spans="3:12" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="25" spans="3:12" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="26" spans="3:12" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C4:G4"/>
+    <mergeCell ref="H4:L4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update script and table 1 (one mistake corrected)
</commit_message>
<xml_diff>
--- a/Tables_v1.xlsx
+++ b/Tables_v1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jgippet\Documents\Tmagnum_impacts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8B49D5E-0629-4973-B6B1-1286803E7CC8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81B03819-EB57-4169-A2C9-2B61B0908C2B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-8325" windowWidth="15600" windowHeight="18840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1172,9 +1172,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1297,39 +1294,6 @@
     <xf numFmtId="0" fontId="18" fillId="5" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1352,6 +1316,42 @@
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1677,8 +1677,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R12"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="T6" sqref="T6"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.8" x14ac:dyDescent="0.4"/>
@@ -1695,42 +1695,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.4">
       <c r="B2" s="3"/>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="42"/>
-      <c r="G2" s="42"/>
-      <c r="H2" s="42"/>
-      <c r="I2" s="42"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="41"/>
+      <c r="I2" s="41"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.4">
       <c r="B3" s="3"/>
-      <c r="C3" s="42"/>
-      <c r="D3" s="42"/>
-      <c r="E3" s="42"/>
-      <c r="F3" s="42"/>
-      <c r="G3" s="42"/>
-      <c r="H3" s="42"/>
-      <c r="I3" s="42"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="41"/>
+      <c r="G3" s="41"/>
+      <c r="H3" s="41"/>
+      <c r="I3" s="41"/>
     </row>
     <row r="4" spans="1:18" ht="16.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C4" s="43"/>
-      <c r="D4" s="43"/>
-      <c r="E4" s="43"/>
-      <c r="F4" s="43"/>
-      <c r="G4" s="43"/>
-      <c r="H4" s="43"/>
-      <c r="I4" s="43"/>
+      <c r="C4" s="42"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="42"/>
+      <c r="F4" s="42"/>
+      <c r="G4" s="42"/>
+      <c r="H4" s="42"/>
+      <c r="I4" s="42"/>
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
@@ -1741,52 +1741,52 @@
       <c r="Q4" s="3"/>
     </row>
     <row r="5" spans="1:18" ht="27.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C5" s="82" t="s">
+      <c r="C5" s="90" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="83"/>
-      <c r="E5" s="83"/>
-      <c r="F5" s="83"/>
-      <c r="G5" s="83"/>
-      <c r="H5" s="83"/>
-      <c r="I5" s="84"/>
-      <c r="J5" s="39"/>
-      <c r="K5" s="82" t="s">
+      <c r="D5" s="91"/>
+      <c r="E5" s="91"/>
+      <c r="F5" s="91"/>
+      <c r="G5" s="91"/>
+      <c r="H5" s="91"/>
+      <c r="I5" s="92"/>
+      <c r="J5" s="38"/>
+      <c r="K5" s="90" t="s">
         <v>10</v>
       </c>
-      <c r="L5" s="83"/>
-      <c r="M5" s="83"/>
-      <c r="N5" s="83"/>
-      <c r="O5" s="83"/>
-      <c r="P5" s="83"/>
-      <c r="Q5" s="84"/>
+      <c r="L5" s="91"/>
+      <c r="M5" s="91"/>
+      <c r="N5" s="91"/>
+      <c r="O5" s="91"/>
+      <c r="P5" s="91"/>
+      <c r="Q5" s="92"/>
     </row>
     <row r="6" spans="1:18" ht="106.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A6" s="80"/>
-      <c r="B6" s="81"/>
-      <c r="C6" s="44" t="s">
+      <c r="A6" s="88"/>
+      <c r="B6" s="89"/>
+      <c r="C6" s="43" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="45" t="s">
+      <c r="D6" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="E6" s="46" t="s">
+      <c r="E6" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="F6" s="47" t="s">
+      <c r="F6" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="G6" s="48" t="s">
+      <c r="G6" s="47" t="s">
         <v>28</v>
       </c>
-      <c r="H6" s="46" t="s">
+      <c r="H6" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="I6" s="99" t="s">
+      <c r="I6" s="87" t="s">
         <v>25</v>
       </c>
       <c r="J6" s="30"/>
-      <c r="K6" s="44" t="s">
+      <c r="K6" s="43" t="s">
         <v>26</v>
       </c>
       <c r="L6" s="27" t="s">
@@ -1795,42 +1795,42 @@
       <c r="M6" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="N6" s="47" t="s">
+      <c r="N6" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="O6" s="48" t="s">
+      <c r="O6" s="47" t="s">
         <v>28</v>
       </c>
       <c r="P6" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="Q6" s="99" t="s">
+      <c r="Q6" s="87" t="s">
         <v>25</v>
       </c>
-      <c r="R6" s="49"/>
+      <c r="R6" s="48"/>
     </row>
     <row r="7" spans="1:18" s="2" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A7" s="4"/>
       <c r="B7" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="93"/>
+      <c r="C7" s="81"/>
       <c r="D7" s="18"/>
       <c r="E7" s="14"/>
-      <c r="F7" s="94"/>
-      <c r="G7" s="94"/>
+      <c r="F7" s="82"/>
+      <c r="G7" s="82"/>
       <c r="H7" s="24"/>
-      <c r="I7" s="96" t="s">
+      <c r="I7" s="84" t="s">
         <v>8</v>
       </c>
-      <c r="J7" s="38"/>
-      <c r="K7" s="95"/>
+      <c r="J7" s="37"/>
+      <c r="K7" s="83"/>
       <c r="L7" s="14"/>
       <c r="M7" s="18"/>
-      <c r="N7" s="94"/>
-      <c r="O7" s="94"/>
+      <c r="N7" s="82"/>
+      <c r="O7" s="82"/>
       <c r="P7" s="22"/>
-      <c r="Q7" s="96" t="s">
+      <c r="Q7" s="84" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1845,17 +1845,17 @@
       <c r="F8" s="21"/>
       <c r="G8" s="15"/>
       <c r="H8" s="25"/>
-      <c r="I8" s="97" t="s">
+      <c r="I8" s="85" t="s">
         <v>24</v>
       </c>
-      <c r="J8" s="38"/>
+      <c r="J8" s="37"/>
       <c r="K8" s="26"/>
       <c r="L8" s="15"/>
       <c r="M8" s="15"/>
       <c r="N8" s="15"/>
-      <c r="O8" s="21"/>
-      <c r="P8" s="37"/>
-      <c r="Q8" s="97" t="s">
+      <c r="O8" s="15"/>
+      <c r="P8" s="99"/>
+      <c r="Q8" s="85" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1870,7 +1870,7 @@
       <c r="F9" s="19"/>
       <c r="G9" s="19"/>
       <c r="H9" s="32"/>
-      <c r="I9" s="97" t="s">
+      <c r="I9" s="85" t="s">
         <v>24</v>
       </c>
       <c r="J9" s="4"/>
@@ -1879,8 +1879,8 @@
       <c r="M9" s="16"/>
       <c r="N9" s="19"/>
       <c r="O9" s="21"/>
-      <c r="P9" s="40"/>
-      <c r="Q9" s="97" t="s">
+      <c r="P9" s="39"/>
+      <c r="Q9" s="85" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1895,7 +1895,7 @@
       <c r="F10" s="19"/>
       <c r="G10" s="19"/>
       <c r="H10" s="34"/>
-      <c r="I10" s="97" t="s">
+      <c r="I10" s="85" t="s">
         <v>23</v>
       </c>
       <c r="J10" s="4"/>
@@ -1905,7 +1905,7 @@
       <c r="N10" s="19"/>
       <c r="O10" s="19"/>
       <c r="P10" s="34"/>
-      <c r="Q10" s="97" t="s">
+      <c r="Q10" s="85" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1920,7 +1920,7 @@
       <c r="F11" s="20"/>
       <c r="G11" s="20"/>
       <c r="H11" s="31"/>
-      <c r="I11" s="98" t="s">
+      <c r="I11" s="86" t="s">
         <v>22</v>
       </c>
       <c r="J11" s="23"/>
@@ -1929,17 +1929,17 @@
       <c r="M11" s="20"/>
       <c r="N11" s="20"/>
       <c r="O11" s="20"/>
-      <c r="P11" s="41"/>
-      <c r="Q11" s="98" t="s">
+      <c r="P11" s="40"/>
+      <c r="Q11" s="86" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.4">
       <c r="B12" s="3"/>
-      <c r="I12" s="92"/>
+      <c r="I12" s="80"/>
       <c r="J12" s="2"/>
       <c r="M12" s="3"/>
-      <c r="Q12" s="91"/>
+      <c r="Q12" s="79"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1958,417 +1958,417 @@
   <dimension ref="B3:L26"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6:G6"/>
+      <selection activeCell="G9" sqref="C9:G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="50"/>
-    <col min="2" max="2" width="16.6640625" style="50" customWidth="1"/>
-    <col min="3" max="12" width="14.21875" style="50" customWidth="1"/>
-    <col min="13" max="16384" width="8.88671875" style="50"/>
+    <col min="1" max="1" width="8.88671875" style="49"/>
+    <col min="2" max="2" width="16.6640625" style="49" customWidth="1"/>
+    <col min="3" max="12" width="14.21875" style="49" customWidth="1"/>
+    <col min="13" max="16384" width="8.88671875" style="49"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C4" s="85" t="s">
+      <c r="C4" s="93" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="86"/>
-      <c r="E4" s="86"/>
-      <c r="F4" s="86"/>
-      <c r="G4" s="87"/>
-      <c r="H4" s="88" t="s">
+      <c r="D4" s="94"/>
+      <c r="E4" s="94"/>
+      <c r="F4" s="94"/>
+      <c r="G4" s="95"/>
+      <c r="H4" s="96" t="s">
         <v>19</v>
       </c>
-      <c r="I4" s="89"/>
-      <c r="J4" s="89"/>
-      <c r="K4" s="89"/>
-      <c r="L4" s="90"/>
+      <c r="I4" s="97"/>
+      <c r="J4" s="97"/>
+      <c r="K4" s="97"/>
+      <c r="L4" s="98"/>
     </row>
-    <row r="5" spans="2:12" s="51" customFormat="1" ht="12" x14ac:dyDescent="0.3">
-      <c r="C5" s="52" t="s">
+    <row r="5" spans="2:12" s="50" customFormat="1" ht="12" x14ac:dyDescent="0.3">
+      <c r="C5" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="53" t="s">
+      <c r="D5" s="52" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="53" t="s">
+      <c r="E5" s="52" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="53" t="s">
+      <c r="F5" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="G5" s="54" t="s">
+      <c r="G5" s="53" t="s">
         <v>20</v>
       </c>
-      <c r="H5" s="55" t="s">
+      <c r="H5" s="54" t="s">
         <v>15</v>
       </c>
-      <c r="I5" s="53" t="s">
+      <c r="I5" s="52" t="s">
         <v>16</v>
       </c>
-      <c r="J5" s="53" t="s">
+      <c r="J5" s="52" t="s">
         <v>17</v>
       </c>
-      <c r="K5" s="53" t="s">
+      <c r="K5" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="L5" s="56" t="s">
+      <c r="L5" s="55" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="6" spans="2:12" ht="18" x14ac:dyDescent="0.3">
-      <c r="B6" s="57" t="s">
+      <c r="B6" s="56" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="76">
+      <c r="C6" s="75">
         <v>267</v>
       </c>
-      <c r="D6" s="61">
+      <c r="D6" s="60">
         <v>25</v>
       </c>
-      <c r="E6" s="61">
-        <v>0</v>
-      </c>
-      <c r="F6" s="61">
+      <c r="E6" s="60">
+        <v>0</v>
+      </c>
+      <c r="F6" s="60">
         <v>1</v>
       </c>
-      <c r="G6" s="62">
+      <c r="G6" s="61">
         <v>6</v>
       </c>
-      <c r="H6" s="75">
+      <c r="H6" s="74">
         <v>257</v>
       </c>
-      <c r="I6" s="61">
+      <c r="I6" s="60">
         <v>13</v>
       </c>
-      <c r="J6" s="61">
+      <c r="J6" s="60">
         <v>2</v>
       </c>
-      <c r="K6" s="61">
+      <c r="K6" s="60">
         <v>1</v>
       </c>
-      <c r="L6" s="64">
+      <c r="L6" s="63">
         <v>6</v>
       </c>
     </row>
     <row r="7" spans="2:12" ht="18" x14ac:dyDescent="0.3">
-      <c r="B7" s="57" t="s">
+      <c r="B7" s="56" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="60">
+      <c r="C7" s="59">
         <v>25</v>
       </c>
-      <c r="D7" s="74">
+      <c r="D7" s="73">
         <v>66</v>
       </c>
-      <c r="E7" s="61">
+      <c r="E7" s="60">
         <v>1</v>
       </c>
-      <c r="F7" s="61">
-        <v>0</v>
-      </c>
-      <c r="G7" s="62">
+      <c r="F7" s="60">
+        <v>0</v>
+      </c>
+      <c r="G7" s="61">
         <v>3</v>
       </c>
-      <c r="H7" s="63">
+      <c r="H7" s="62">
         <v>13</v>
       </c>
-      <c r="I7" s="74">
+      <c r="I7" s="73">
         <v>15</v>
       </c>
-      <c r="J7" s="61">
-        <v>0</v>
-      </c>
-      <c r="K7" s="61">
-        <v>0</v>
-      </c>
-      <c r="L7" s="64">
+      <c r="J7" s="60">
+        <v>0</v>
+      </c>
+      <c r="K7" s="60">
+        <v>0</v>
+      </c>
+      <c r="L7" s="63">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="2:12" ht="18" x14ac:dyDescent="0.3">
-      <c r="B8" s="57" t="s">
+      <c r="B8" s="56" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="60">
-        <v>0</v>
-      </c>
-      <c r="D8" s="61">
+      <c r="C8" s="59">
+        <v>0</v>
+      </c>
+      <c r="D8" s="60">
         <v>1</v>
       </c>
-      <c r="E8" s="74">
+      <c r="E8" s="73">
         <v>71</v>
       </c>
-      <c r="F8" s="61">
-        <v>0</v>
-      </c>
-      <c r="G8" s="62">
+      <c r="F8" s="60">
+        <v>0</v>
+      </c>
+      <c r="G8" s="61">
         <v>2</v>
       </c>
-      <c r="H8" s="63">
+      <c r="H8" s="62">
         <v>2</v>
       </c>
-      <c r="I8" s="61">
-        <v>0</v>
-      </c>
-      <c r="J8" s="74">
+      <c r="I8" s="60">
+        <v>0</v>
+      </c>
+      <c r="J8" s="73">
         <v>7</v>
       </c>
-      <c r="K8" s="61">
-        <v>0</v>
-      </c>
-      <c r="L8" s="64">
+      <c r="K8" s="60">
+        <v>0</v>
+      </c>
+      <c r="L8" s="63">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="2:12" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="58" t="s">
+      <c r="B9" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="65">
+      <c r="C9" s="64">
         <v>1</v>
       </c>
-      <c r="D9" s="66">
-        <v>0</v>
-      </c>
-      <c r="E9" s="66">
-        <v>0</v>
-      </c>
-      <c r="F9" s="73">
+      <c r="D9" s="65">
+        <v>0</v>
+      </c>
+      <c r="E9" s="65">
+        <v>0</v>
+      </c>
+      <c r="F9" s="72">
         <v>58</v>
       </c>
-      <c r="G9" s="67">
+      <c r="G9" s="66">
         <v>1</v>
       </c>
-      <c r="H9" s="68">
+      <c r="H9" s="67">
         <v>1</v>
       </c>
-      <c r="I9" s="66">
-        <v>0</v>
-      </c>
-      <c r="J9" s="66">
-        <v>0</v>
-      </c>
-      <c r="K9" s="73">
+      <c r="I9" s="65">
+        <v>0</v>
+      </c>
+      <c r="J9" s="65">
+        <v>0</v>
+      </c>
+      <c r="K9" s="72">
         <v>15</v>
       </c>
-      <c r="L9" s="69">
+      <c r="L9" s="68">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="2:12" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="59" t="s">
+      <c r="B10" s="58" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="70"/>
-      <c r="D10" s="71"/>
-      <c r="E10" s="71"/>
-      <c r="F10" s="71"/>
-      <c r="G10" s="72"/>
-      <c r="H10" s="77">
+      <c r="C10" s="69"/>
+      <c r="D10" s="70"/>
+      <c r="E10" s="70"/>
+      <c r="F10" s="70"/>
+      <c r="G10" s="71"/>
+      <c r="H10" s="76">
         <v>8</v>
       </c>
-      <c r="I10" s="78">
+      <c r="I10" s="77">
         <v>8</v>
       </c>
-      <c r="J10" s="78">
+      <c r="J10" s="77">
         <v>1</v>
       </c>
-      <c r="K10" s="78">
-        <v>0</v>
-      </c>
-      <c r="L10" s="79">
+      <c r="K10" s="77">
+        <v>0</v>
+      </c>
+      <c r="L10" s="78">
         <v>4</v>
       </c>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="C14" s="50">
+      <c r="C14" s="49">
         <f>ROUND(C6/960,2)</f>
         <v>0.28000000000000003</v>
       </c>
-      <c r="D14" s="50">
+      <c r="D14" s="49">
         <f t="shared" ref="D14:G14" si="0">ROUND(D6/960,2)</f>
         <v>0.03</v>
       </c>
-      <c r="E14" s="50">
+      <c r="E14" s="49">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F14" s="50">
+      <c r="F14" s="49">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G14" s="50">
+      <c r="G14" s="49">
         <f t="shared" si="0"/>
         <v>0.01</v>
       </c>
-      <c r="H14" s="50">
+      <c r="H14" s="49">
         <f>ROUND(H6/960,2)</f>
         <v>0.27</v>
       </c>
-      <c r="I14" s="50">
+      <c r="I14" s="49">
         <f t="shared" ref="I14:L14" si="1">ROUND(I6/960,2)</f>
         <v>0.01</v>
       </c>
-      <c r="J14" s="50">
+      <c r="J14" s="49">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K14" s="50">
+      <c r="K14" s="49">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L14" s="50">
+      <c r="L14" s="49">
         <f t="shared" si="1"/>
         <v>0.01</v>
       </c>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="C15" s="50">
+      <c r="C15" s="49">
         <f t="shared" ref="C15:G15" si="2">ROUND(C7/960,2)</f>
         <v>0.03</v>
       </c>
-      <c r="D15" s="50">
+      <c r="D15" s="49">
         <f t="shared" si="2"/>
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="E15" s="50">
+      <c r="E15" s="49">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F15" s="50">
+      <c r="F15" s="49">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G15" s="50">
+      <c r="G15" s="49">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H15" s="50">
+      <c r="H15" s="49">
         <f t="shared" ref="H15:L15" si="3">ROUND(H7/960,2)</f>
         <v>0.01</v>
       </c>
-      <c r="I15" s="50">
+      <c r="I15" s="49">
         <f t="shared" si="3"/>
         <v>0.02</v>
       </c>
-      <c r="J15" s="50">
+      <c r="J15" s="49">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="K15" s="50">
+      <c r="K15" s="49">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="L15" s="50">
+      <c r="L15" s="49">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="C16" s="50">
+      <c r="C16" s="49">
         <f t="shared" ref="C16:G16" si="4">ROUND(C8/960,2)</f>
         <v>0</v>
       </c>
-      <c r="D16" s="50">
+      <c r="D16" s="49">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="E16" s="50">
+      <c r="E16" s="49">
         <f t="shared" si="4"/>
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="F16" s="50">
+      <c r="F16" s="49">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="G16" s="50">
+      <c r="G16" s="49">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="H16" s="50">
+      <c r="H16" s="49">
         <f t="shared" ref="H16:L16" si="5">ROUND(H8/960,2)</f>
         <v>0</v>
       </c>
-      <c r="I16" s="50">
+      <c r="I16" s="49">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="J16" s="50">
+      <c r="J16" s="49">
         <f t="shared" si="5"/>
         <v>0.01</v>
       </c>
-      <c r="K16" s="50">
+      <c r="K16" s="49">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="L16" s="50">
+      <c r="L16" s="49">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C17" s="50">
+      <c r="C17" s="49">
         <f t="shared" ref="C17:G17" si="6">ROUND(C9/960,2)</f>
         <v>0</v>
       </c>
-      <c r="D17" s="50">
+      <c r="D17" s="49">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="E17" s="50">
+      <c r="E17" s="49">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="F17" s="50">
+      <c r="F17" s="49">
         <f t="shared" si="6"/>
         <v>0.06</v>
       </c>
-      <c r="G17" s="50">
+      <c r="G17" s="49">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="H17" s="50">
+      <c r="H17" s="49">
         <f t="shared" ref="H17:L18" si="7">ROUND(H9/960,2)</f>
         <v>0</v>
       </c>
-      <c r="I17" s="50">
+      <c r="I17" s="49">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="J17" s="50">
+      <c r="J17" s="49">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="K17" s="50">
+      <c r="K17" s="49">
         <f t="shared" si="7"/>
         <v>0.02</v>
       </c>
-      <c r="L17" s="50">
+      <c r="L17" s="49">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="H18" s="50">
+      <c r="H18" s="49">
         <f>ROUND(H10/960,2)</f>
         <v>0.01</v>
       </c>
-      <c r="I18" s="50">
+      <c r="I18" s="49">
         <f t="shared" si="7"/>
         <v>0.01</v>
       </c>
-      <c r="J18" s="50">
+      <c r="J18" s="49">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="K18" s="50">
+      <c r="K18" s="49">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="L18" s="50">
+      <c r="L18" s="49">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>

</xml_diff>